<commit_message>
Completed the Driver Code and Created test CSV File for ISE Faculty
</commit_message>
<xml_diff>
--- a/ISE/FACULTY/ise_faculty.xlsx
+++ b/ISE/FACULTY/ise_faculty.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/814fd49cbebc9953/Desktop/code/Campus-Vaccination-Management-System/ISE/FACULTY/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC1048CAF91A6FEC5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37519055-381D-4254-9F4C-E85D2D3EE183}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>FSN</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Shamanth</t>
+  </si>
+  <si>
+    <t>FID1</t>
+  </si>
+  <si>
+    <t>FID2</t>
+  </si>
+  <si>
+    <t>Naveen</t>
+  </si>
+  <si>
+    <t>FID3</t>
+  </si>
+  <si>
+    <t>Ganaraj</t>
+  </si>
+  <si>
+    <t>FID4</t>
+  </si>
+  <si>
+    <t>Madhura</t>
+  </si>
+  <si>
+    <t>FID5</t>
+  </si>
+  <si>
+    <t>Jayapadmini</t>
+  </si>
+  <si>
+    <t>FID6</t>
+  </si>
+  <si>
+    <t>Asha</t>
+  </si>
+  <si>
+    <t>FID7</t>
+  </si>
+  <si>
+    <t>Shwetha</t>
+  </si>
+  <si>
+    <t>FID8</t>
+  </si>
+  <si>
+    <t>Rithesh</t>
+  </si>
+  <si>
+    <t>FID9</t>
+  </si>
+  <si>
+    <t>Naitik</t>
+  </si>
+  <si>
+    <t>FID10</t>
+  </si>
+  <si>
+    <t>Vasudev</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,8 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +427,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9986407821</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9743750743</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8086714071</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9986429412</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9535667372</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9483015748</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2">
+        <v>9449330933</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2">
+        <v>9449389449</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8296502878</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8217894079</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>